<commit_message>
fix bug duplicate dash board
</commit_message>
<xml_diff>
--- a/WahoClient/wwwroot/InventoryDetail.xlsx
+++ b/WahoClient/wwwroot/InventoryDetail.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Mã phiếu kiểm kho :</t>
   </si>
@@ -20,19 +20,19 @@
     <t>Người kiểm phiếu</t>
   </si>
   <si>
-    <t>Trần Văn Đức</t>
+    <t>Chi Tùng</t>
   </si>
   <si>
     <t>Ngày tạo</t>
   </si>
   <si>
-    <t>15/6/2023 12:00:00 AM</t>
+    <t>21/7/2023 12:00:00 AM</t>
   </si>
   <si>
     <t>Tổng tiền chênh</t>
   </si>
   <si>
-    <t>4650000 đồng</t>
+    <t>-35500000 đồng</t>
   </si>
   <si>
     <t>Tên sản phẩm</t>
@@ -60,6 +60,54 @@
   </si>
   <si>
     <t>Phông Be</t>
+  </si>
+  <si>
+    <t>Phông Trắng</t>
+  </si>
+  <si>
+    <t>Phông Đen</t>
+  </si>
+  <si>
+    <t>Phông Hoa</t>
+  </si>
+  <si>
+    <t>Phông Logo</t>
+  </si>
+  <si>
+    <t>Phông Hồng</t>
+  </si>
+  <si>
+    <t>Phông Xám</t>
+  </si>
+  <si>
+    <t>test create</t>
+  </si>
+  <si>
+    <t>test create 2 update</t>
+  </si>
+  <si>
+    <t>Áo Khoác hồng</t>
+  </si>
+  <si>
+    <t>Áo Khoác hồng ver 2</t>
+  </si>
+  <si>
+    <t>áo Tshirt ong mật ver 7</t>
+  </si>
+  <si>
+    <t>áo Tshirt ong mật ver 2</t>
+  </si>
+  <si>
+    <t>Áo Khoác hồng ver 3</t>
+  </si>
+  <si>
+    <t>Áo Khoác hồng ver 4</t>
+  </si>
+  <si>
+    <t>áo Tshirt ong mật ver 5</t>
+  </si>
+  <si>
+    <t>áo Tshirt ong mật ver 6</t>
   </si>
 </sst>
 </file>
@@ -105,7 +153,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -116,7 +164,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2">
@@ -165,16 +213,16 @@
         <v>12</v>
       </c>
       <c r="B6" s="0">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C6" s="0">
         <v>89</v>
       </c>
       <c r="D6" s="0">
-        <v>10</v>
+        <v>-49</v>
       </c>
       <c r="E6" s="0">
-        <v>1500000</v>
+        <v>-7350000</v>
       </c>
     </row>
     <row r="7">
@@ -182,16 +230,16 @@
         <v>13</v>
       </c>
       <c r="B7" s="0">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="C7" s="0">
         <v>89</v>
       </c>
       <c r="D7" s="0">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="E7" s="0">
-        <v>3300000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="8">
@@ -199,16 +247,16 @@
         <v>14</v>
       </c>
       <c r="B8" s="0">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="C8" s="0">
         <v>100</v>
       </c>
       <c r="D8" s="0">
-        <v>-11</v>
+        <v>0</v>
       </c>
       <c r="E8" s="0">
-        <v>-1650000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -226,6 +274,278 @@
       </c>
       <c r="E9" s="0">
         <v>1500000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="0">
+        <v>100</v>
+      </c>
+      <c r="C10" s="0">
+        <v>100</v>
+      </c>
+      <c r="D10" s="0">
+        <v>0</v>
+      </c>
+      <c r="E10" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="0">
+        <v>100</v>
+      </c>
+      <c r="C11" s="0">
+        <v>100</v>
+      </c>
+      <c r="D11" s="0">
+        <v>0</v>
+      </c>
+      <c r="E11" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="0">
+        <v>90</v>
+      </c>
+      <c r="C12" s="0">
+        <v>90</v>
+      </c>
+      <c r="D12" s="0">
+        <v>0</v>
+      </c>
+      <c r="E12" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="0">
+        <v>100</v>
+      </c>
+      <c r="C13" s="0">
+        <v>100</v>
+      </c>
+      <c r="D13" s="0">
+        <v>0</v>
+      </c>
+      <c r="E13" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="0">
+        <v>100</v>
+      </c>
+      <c r="C14" s="0">
+        <v>100</v>
+      </c>
+      <c r="D14" s="0">
+        <v>0</v>
+      </c>
+      <c r="E14" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="0">
+        <v>100</v>
+      </c>
+      <c r="C15" s="0">
+        <v>100</v>
+      </c>
+      <c r="D15" s="0">
+        <v>0</v>
+      </c>
+      <c r="E15" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="0">
+        <v>988</v>
+      </c>
+      <c r="C16" s="0">
+        <v>988</v>
+      </c>
+      <c r="D16" s="0">
+        <v>0</v>
+      </c>
+      <c r="E16" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="0">
+        <v>99</v>
+      </c>
+      <c r="C17" s="0">
+        <v>98</v>
+      </c>
+      <c r="D17" s="0">
+        <v>1</v>
+      </c>
+      <c r="E17" s="0">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="0">
+        <v>100</v>
+      </c>
+      <c r="C18" s="0">
+        <v>200</v>
+      </c>
+      <c r="D18" s="0">
+        <v>-100</v>
+      </c>
+      <c r="E18" s="0">
+        <v>-30000000</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="0">
+        <v>200</v>
+      </c>
+      <c r="C19" s="0">
+        <v>200</v>
+      </c>
+      <c r="D19" s="0">
+        <v>0</v>
+      </c>
+      <c r="E19" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="0">
+        <v>200</v>
+      </c>
+      <c r="C20" s="0">
+        <v>200</v>
+      </c>
+      <c r="D20" s="0">
+        <v>0</v>
+      </c>
+      <c r="E20" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="0">
+        <v>200</v>
+      </c>
+      <c r="C21" s="0">
+        <v>200</v>
+      </c>
+      <c r="D21" s="0">
+        <v>0</v>
+      </c>
+      <c r="E21" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="0">
+        <v>200</v>
+      </c>
+      <c r="C22" s="0">
+        <v>200</v>
+      </c>
+      <c r="D22" s="0">
+        <v>0</v>
+      </c>
+      <c r="E22" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="0">
+        <v>200</v>
+      </c>
+      <c r="C23" s="0">
+        <v>200</v>
+      </c>
+      <c r="D23" s="0">
+        <v>0</v>
+      </c>
+      <c r="E23" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="0">
+        <v>200</v>
+      </c>
+      <c r="C24" s="0">
+        <v>200</v>
+      </c>
+      <c r="D24" s="0">
+        <v>0</v>
+      </c>
+      <c r="E24" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="0">
+        <v>200</v>
+      </c>
+      <c r="C25" s="0">
+        <v>200</v>
+      </c>
+      <c r="D25" s="0">
+        <v>0</v>
+      </c>
+      <c r="E25" s="0">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>